<commit_message>
Changed cell colors on days that we were at the sites. Created new rows to determine the number of samples we would have after removing those sample dates.
</commit_message>
<xml_diff>
--- a/Project_Plan/Analysis_Time_Worksheet.xlsx
+++ b/Project_Plan/Analysis_Time_Worksheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="707" documentId="11_F25DC773A252ABEACE02ECC5AB5E572A5ADE589F" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{6A3160D6-6AF6-4B75-9A38-ED319A6337F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C923C7B5-1DB7-4923-9917-19B5D84E33FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Sound Analysis Time</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>Total number of samples under each sampling method</t>
+  </si>
+  <si>
+    <t>Number of recordings - removed recordings</t>
+  </si>
+  <si>
+    <t>Number of recordings removed for divers that day</t>
   </si>
 </sst>
 </file>
@@ -211,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,8 +314,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="37">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -388,17 +400,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -540,21 +541,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -751,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -773,78 +759,174 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="11" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -856,132 +938,39 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1271,13 +1260,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.53125" customWidth="1"/>
     <col min="2" max="2" width="17.06640625" customWidth="1"/>
     <col min="3" max="3" width="13.19921875" customWidth="1"/>
     <col min="4" max="4" width="14.06640625" customWidth="1"/>
@@ -1292,158 +1281,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="62" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="62" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="114"/>
-      <c r="C4" s="114"/>
-      <c r="D4" s="114"/>
-      <c r="E4" s="114"/>
-      <c r="F4" s="114"/>
-      <c r="G4" s="114"/>
-      <c r="H4" s="114"/>
-      <c r="I4" s="114"/>
-      <c r="J4" s="114"/>
-      <c r="K4" s="114"/>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="114"/>
-      <c r="O4" s="114"/>
-      <c r="P4" s="114"/>
-      <c r="Q4" s="114"/>
-      <c r="R4" s="114"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="101"/>
+      <c r="P4" s="101"/>
+      <c r="Q4" s="101"/>
+      <c r="R4" s="101"/>
       <c r="S4" s="10"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="114"/>
-      <c r="B5" s="114"/>
-      <c r="C5" s="114"/>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
-      <c r="P5" s="114"/>
-      <c r="Q5" s="114"/>
-      <c r="R5" s="114"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="101"/>
+      <c r="Q5" s="101"/>
+      <c r="R5" s="101"/>
       <c r="S5" s="10"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="114"/>
-      <c r="B6" s="114"/>
-      <c r="C6" s="114"/>
-      <c r="D6" s="114"/>
-      <c r="E6" s="114"/>
-      <c r="F6" s="114"/>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="114"/>
-      <c r="L6" s="114"/>
-      <c r="M6" s="114"/>
-      <c r="N6" s="114"/>
-      <c r="O6" s="114"/>
-      <c r="P6" s="114"/>
-      <c r="Q6" s="114"/>
-      <c r="R6" s="114"/>
+      <c r="A6" s="101"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="101"/>
+      <c r="N6" s="101"/>
+      <c r="O6" s="101"/>
+      <c r="P6" s="101"/>
+      <c r="Q6" s="101"/>
+      <c r="R6" s="101"/>
       <c r="S6" s="10"/>
     </row>
-    <row r="7" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="114"/>
-      <c r="B7" s="114"/>
-      <c r="C7" s="114"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="114"/>
-      <c r="I7" s="114"/>
-      <c r="J7" s="114"/>
-      <c r="K7" s="114"/>
-      <c r="L7" s="114"/>
-      <c r="M7" s="114"/>
-      <c r="N7" s="114"/>
-      <c r="O7" s="114"/>
-      <c r="P7" s="114"/>
-      <c r="Q7" s="114"/>
-      <c r="R7" s="114"/>
+    <row r="7" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="101"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
+      <c r="N7" s="101"/>
+      <c r="O7" s="101"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="101"/>
       <c r="S7" s="10"/>
     </row>
     <row r="8" spans="1:20" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="115"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="116"/>
-      <c r="J8" s="117" t="s">
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="117"/>
-      <c r="L8" s="117"/>
-      <c r="M8" s="118"/>
-      <c r="N8" s="119" t="s">
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="O8" s="120"/>
-      <c r="P8" s="120"/>
-      <c r="Q8" s="121"/>
-      <c r="R8" s="122"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="109"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="67"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="123" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="3">
@@ -1452,30 +1441,30 @@
       <c r="C9" s="1">
         <v>45</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="124">
         <v>65</v>
       </c>
-      <c r="E9" s="123"/>
-      <c r="F9" s="62"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="55"/>
       <c r="G9" s="37"/>
-      <c r="H9" s="82" t="s">
+      <c r="H9" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="82"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="108"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="77"/>
-      <c r="P9" s="77"/>
-      <c r="Q9" s="78"/>
+      <c r="I9" s="87"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="111"/>
+      <c r="O9" s="112"/>
+      <c r="P9" s="112"/>
+      <c r="Q9" s="113"/>
       <c r="R9" s="35"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="125" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="3">
@@ -1484,7 +1473,7 @@
       <c r="C10" s="2">
         <v>4</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="124">
         <v>4</v>
       </c>
       <c r="E10" s="10"/>
@@ -1506,20 +1495,20 @@
       <c r="K10" s="13">
         <v>40</v>
       </c>
-      <c r="L10" s="96" t="s">
+      <c r="L10" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="97"/>
-      <c r="N10" s="54" t="s">
+      <c r="M10" s="83"/>
+      <c r="N10" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="55" t="s">
+      <c r="O10" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="56" t="s">
+      <c r="P10" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="101" t="s">
+      <c r="Q10" s="60" t="s">
         <v>36</v>
       </c>
       <c r="R10" s="10"/>
@@ -1527,7 +1516,7 @@
       <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="125" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="3">
@@ -1538,7 +1527,7 @@
         <f>C9*C10</f>
         <v>180</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="124">
         <f>D9*D10</f>
         <v>260</v>
       </c>
@@ -1561,11 +1550,11 @@
       <c r="K11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="98" t="s">
+      <c r="L11" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="99"/>
-      <c r="N11" s="58">
+      <c r="M11" s="85"/>
+      <c r="N11" s="51">
         <v>2017</v>
       </c>
       <c r="O11" s="4">
@@ -1574,7 +1563,7 @@
       <c r="P11" s="7">
         <v>25</v>
       </c>
-      <c r="Q11" s="57">
+      <c r="Q11" s="50">
         <v>40</v>
       </c>
       <c r="R11" s="10"/>
@@ -1582,31 +1571,31 @@
       <c r="T11" s="10"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A12" s="49" t="s">
-        <v>2</v>
+      <c r="A12" s="125" t="s">
+        <v>42</v>
       </c>
       <c r="B12" s="3">
-        <f>B11/40</f>
-        <v>3</v>
-      </c>
-      <c r="C12" s="2">
-        <f>C11/40</f>
-        <v>4.5</v>
-      </c>
-      <c r="D12" s="48">
-        <f>D11/40</f>
-        <v>6.5</v>
+        <f>3*4</f>
+        <v>12</v>
+      </c>
+      <c r="C12" s="126">
+        <f>9*4</f>
+        <v>36</v>
+      </c>
+      <c r="D12" s="124">
+        <f>9*4</f>
+        <v>36</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="111"/>
-      <c r="L12" s="112"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="65"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="58">
+      <c r="N12" s="51">
         <v>2018</v>
       </c>
       <c r="O12" s="4">
@@ -1615,38 +1604,41 @@
       <c r="P12" s="7">
         <v>20</v>
       </c>
-      <c r="Q12" s="57">
+      <c r="Q12" s="50">
         <v>25</v>
       </c>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
     </row>
-    <row r="13" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="51">
-        <v>43153</v>
-      </c>
-      <c r="C13" s="52">
-        <v>43167</v>
-      </c>
-      <c r="D13" s="53">
-        <v>43181</v>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A13" s="125" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3">
+        <f>B11-B12</f>
+        <v>108</v>
+      </c>
+      <c r="C13" s="126">
+        <f t="shared" ref="C13:D13" si="0">C11-C12</f>
+        <v>144</v>
+      </c>
+      <c r="D13" s="124">
+        <f t="shared" si="0"/>
+        <v>224</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="38"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="83" t="s">
+      <c r="H13" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="83"/>
+      <c r="I13" s="88"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="39"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="59" t="s">
+      <c r="N13" s="52" t="s">
         <v>21</v>
       </c>
       <c r="O13" s="4">
@@ -1655,7 +1647,7 @@
       <c r="P13" s="7">
         <v>45</v>
       </c>
-      <c r="Q13" s="57">
+      <c r="Q13" s="50">
         <v>65</v>
       </c>
       <c r="R13" s="10"/>
@@ -1663,10 +1655,21 @@
       <c r="T13" s="10"/>
     </row>
     <row r="14" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="11"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
+      <c r="A14" s="125" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3">
+        <f>B13/40</f>
+        <v>2.7</v>
+      </c>
+      <c r="C14" s="2">
+        <f>C13/40</f>
+        <v>3.6</v>
+      </c>
+      <c r="D14" s="124">
+        <f>D13/40</f>
+        <v>5.6</v>
+      </c>
       <c r="E14" s="35"/>
       <c r="F14" s="38" t="s">
         <v>15</v>
@@ -1688,7 +1691,7 @@
       </c>
       <c r="L14" s="39"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="60" t="s">
+      <c r="N14" s="53" t="s">
         <v>16</v>
       </c>
       <c r="O14" s="19">
@@ -1699,7 +1702,7 @@
         <f>P13*4</f>
         <v>180</v>
       </c>
-      <c r="Q14" s="61">
+      <c r="Q14" s="54">
         <f>Q13*4</f>
         <v>260</v>
       </c>
@@ -1708,10 +1711,18 @@
       <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="11"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
+      <c r="A15" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="44">
+        <v>43153</v>
+      </c>
+      <c r="C15" s="45">
+        <v>43167</v>
+      </c>
+      <c r="D15" s="46">
+        <v>43181</v>
+      </c>
       <c r="E15" s="35"/>
       <c r="F15" s="40" t="s">
         <v>19</v>
@@ -1731,10 +1742,10 @@
       <c r="K15" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L15" s="98" t="s">
+      <c r="L15" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="100"/>
+      <c r="M15" s="86"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
@@ -1810,109 +1821,109 @@
       <c r="T18" s="10"/>
     </row>
     <row r="19" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="90" t="s">
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="91"/>
-      <c r="I19" s="91"/>
-      <c r="J19" s="91"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="70" t="s">
+      <c r="H19" s="96"/>
+      <c r="I19" s="96"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="M19" s="71"/>
-      <c r="N19" s="71"/>
-      <c r="O19" s="71"/>
-      <c r="P19" s="72"/>
+      <c r="M19" s="103"/>
+      <c r="N19" s="103"/>
+      <c r="O19" s="103"/>
+      <c r="P19" s="104"/>
       <c r="Q19" s="22"/>
       <c r="R19" s="14"/>
       <c r="S19" s="14"/>
       <c r="T19" s="14"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A20" s="64"/>
-      <c r="B20" s="87"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="94"/>
-      <c r="J20" s="94"/>
-      <c r="K20" s="95"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="75"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="92"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="94"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="99"/>
+      <c r="J20" s="99"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="105"/>
+      <c r="M20" s="106"/>
+      <c r="N20" s="106"/>
+      <c r="O20" s="106"/>
+      <c r="P20" s="107"/>
       <c r="Q20" s="23"/>
       <c r="R20" s="14"/>
       <c r="S20" s="14"/>
       <c r="T20" s="14"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A21" s="64"/>
-      <c r="B21" s="87"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="94"/>
-      <c r="J21" s="94"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="75"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="92"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="99"/>
+      <c r="J21" s="99"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="105"/>
+      <c r="M21" s="106"/>
+      <c r="N21" s="106"/>
+      <c r="O21" s="106"/>
+      <c r="P21" s="107"/>
       <c r="Q21" s="23"/>
       <c r="R21" s="14"/>
       <c r="S21" s="14"/>
       <c r="T21" s="14"/>
     </row>
     <row r="22" spans="1:20" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="64"/>
-      <c r="B22" s="67" t="s">
+      <c r="A22" s="57"/>
+      <c r="B22" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="67" t="s">
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="78"/>
+      <c r="G22" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="69"/>
-      <c r="L22" s="67" t="s">
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="77"/>
+      <c r="K22" s="78"/>
+      <c r="L22" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="M22" s="68"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="69"/>
+      <c r="M22" s="77"/>
+      <c r="N22" s="77"/>
+      <c r="O22" s="77"/>
+      <c r="P22" s="78"/>
       <c r="Q22" s="23"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="113">
+      <c r="A23" s="79">
         <v>42917</v>
       </c>
       <c r="B23" s="17">
@@ -1960,7 +1971,7 @@
       <c r="P23" s="12">
         <v>40</v>
       </c>
-      <c r="Q23" s="79" t="s">
+      <c r="Q23" s="114" t="s">
         <v>4</v>
       </c>
       <c r="R23" s="10"/>
@@ -1969,13 +1980,13 @@
     </row>
     <row r="24" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="80"/>
-      <c r="B24" s="65">
+      <c r="B24" s="58">
         <v>11</v>
       </c>
       <c r="C24" s="4">
         <v>11</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="116">
         <v>11</v>
       </c>
       <c r="E24" s="4">
@@ -1987,10 +1998,10 @@
       <c r="G24" s="6">
         <v>11</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="115">
         <v>11</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="115">
         <v>11</v>
       </c>
       <c r="J24" s="7">
@@ -2002,10 +2013,10 @@
       <c r="L24" s="31">
         <v>11</v>
       </c>
-      <c r="M24" s="24">
+      <c r="M24" s="115">
         <v>11</v>
       </c>
-      <c r="N24" s="24">
+      <c r="N24" s="115">
         <v>11</v>
       </c>
       <c r="O24" s="24">
@@ -2014,14 +2025,14 @@
       <c r="P24" s="32">
         <v>11</v>
       </c>
-      <c r="Q24" s="79"/>
+      <c r="Q24" s="114"/>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A25" s="80"/>
-      <c r="B25" s="65">
+      <c r="B25" s="58">
         <v>16</v>
       </c>
       <c r="C25" s="4">
@@ -2033,10 +2044,10 @@
       <c r="E25" s="4">
         <v>16</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="118">
         <v>16</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="117">
         <v>14</v>
       </c>
       <c r="H25" s="7">
@@ -2066,14 +2077,14 @@
       <c r="P25" s="32">
         <v>13</v>
       </c>
-      <c r="Q25" s="79"/>
+      <c r="Q25" s="114"/>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A26" s="80"/>
-      <c r="B26" s="65">
+      <c r="B26" s="58">
         <v>21</v>
       </c>
       <c r="C26" s="4">
@@ -2118,14 +2129,14 @@
       <c r="P26" s="32">
         <v>15</v>
       </c>
-      <c r="Q26" s="79"/>
+      <c r="Q26" s="114"/>
       <c r="R26" s="10"/>
       <c r="S26" s="10"/>
       <c r="T26" s="10"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" s="80"/>
-      <c r="B27" s="65"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -2139,13 +2150,13 @@
       <c r="I27" s="7">
         <v>20</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="115">
         <v>20</v>
       </c>
-      <c r="K27" s="28">
+      <c r="K27" s="118">
         <v>20</v>
       </c>
-      <c r="L27" s="31">
+      <c r="L27" s="117">
         <v>17</v>
       </c>
       <c r="M27" s="24">
@@ -2160,14 +2171,14 @@
       <c r="P27" s="32">
         <v>17</v>
       </c>
-      <c r="Q27" s="79"/>
+      <c r="Q27" s="114"/>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
       <c r="T27" s="10"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A28" s="80"/>
-      <c r="B28" s="65"/>
+      <c r="B28" s="58"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -2175,10 +2186,10 @@
       <c r="G28" s="6">
         <v>23</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="115">
         <v>23</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="115">
         <v>23</v>
       </c>
       <c r="J28" s="7">
@@ -2202,14 +2213,14 @@
       <c r="P28" s="32">
         <v>19</v>
       </c>
-      <c r="Q28" s="79"/>
+      <c r="Q28" s="114"/>
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
       <c r="T28" s="10"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A29" s="80"/>
-      <c r="B29" s="65"/>
+      <c r="B29" s="58"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2234,14 +2245,14 @@
       <c r="P29" s="32">
         <v>21</v>
       </c>
-      <c r="Q29" s="79"/>
+      <c r="Q29" s="114"/>
       <c r="R29" s="10"/>
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
     </row>
     <row r="30" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="80"/>
-      <c r="B30" s="65"/>
+      <c r="B30" s="58"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -2254,10 +2265,10 @@
       <c r="L30" s="31">
         <v>23</v>
       </c>
-      <c r="M30" s="24">
+      <c r="M30" s="115">
         <v>23</v>
       </c>
-      <c r="N30" s="24">
+      <c r="N30" s="115">
         <v>23</v>
       </c>
       <c r="O30" s="24">
@@ -2266,14 +2277,14 @@
       <c r="P30" s="32">
         <v>23</v>
       </c>
-      <c r="Q30" s="79"/>
+      <c r="Q30" s="114"/>
       <c r="R30" s="10"/>
       <c r="S30" s="16"/>
       <c r="T30" s="16"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A31" s="81"/>
-      <c r="B31" s="65"/>
+      <c r="B31" s="58"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2283,7 +2294,7 @@
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="28"/>
-      <c r="L31" s="31">
+      <c r="L31" s="117">
         <v>25</v>
       </c>
       <c r="M31" s="24">
@@ -2298,37 +2309,37 @@
       <c r="P31" s="32">
         <v>25</v>
       </c>
-      <c r="Q31" s="79"/>
+      <c r="Q31" s="114"/>
       <c r="R31" s="10"/>
       <c r="S31" s="10"/>
       <c r="T31" s="10"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A32" s="113">
+      <c r="A32" s="79">
         <v>43252</v>
       </c>
-      <c r="B32" s="67" t="s">
+      <c r="B32" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="68"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="67" t="s">
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="67" t="s">
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="M32" s="68"/>
-      <c r="N32" s="68"/>
-      <c r="O32" s="68"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="66"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="77"/>
+      <c r="P32" s="78"/>
+      <c r="Q32" s="59"/>
       <c r="R32" s="10"/>
       <c r="S32" s="10"/>
       <c r="T32" s="10"/>
@@ -2390,7 +2401,7 @@
       <c r="B34" s="4">
         <v>18</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="115">
         <v>18</v>
       </c>
       <c r="D34" s="4">
@@ -2405,7 +2416,7 @@
       <c r="G34" s="6">
         <v>18</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="115">
         <v>18</v>
       </c>
       <c r="I34" s="7">
@@ -2420,7 +2431,7 @@
       <c r="L34" s="31">
         <v>18</v>
       </c>
-      <c r="M34" s="24">
+      <c r="M34" s="115">
         <v>18</v>
       </c>
       <c r="N34" s="24">
@@ -2429,10 +2440,10 @@
       <c r="O34" s="24">
         <v>18</v>
       </c>
-      <c r="P34" s="32">
+      <c r="P34" s="118">
         <v>18</v>
       </c>
-      <c r="Q34" s="106" t="s">
+      <c r="Q34" s="70" t="s">
         <v>4</v>
       </c>
       <c r="R34" s="21"/>
@@ -2468,7 +2479,7 @@
       <c r="J35" s="7">
         <v>21</v>
       </c>
-      <c r="K35" s="28">
+      <c r="K35" s="118">
         <v>21</v>
       </c>
       <c r="L35" s="31">
@@ -2486,7 +2497,7 @@
       <c r="P35" s="32">
         <v>20</v>
       </c>
-      <c r="Q35" s="106"/>
+      <c r="Q35" s="70"/>
       <c r="R35" s="10"/>
       <c r="S35" s="10"/>
       <c r="T35" s="10"/>
@@ -2513,7 +2524,7 @@
       <c r="K36" s="28">
         <v>24</v>
       </c>
-      <c r="L36" s="31">
+      <c r="L36" s="117">
         <v>22</v>
       </c>
       <c r="M36" s="24">
@@ -2528,7 +2539,7 @@
       <c r="P36" s="32">
         <v>22</v>
       </c>
-      <c r="Q36" s="106"/>
+      <c r="Q36" s="70"/>
       <c r="R36" s="10"/>
       <c r="S36" s="10"/>
       <c r="T36" s="10"/>
@@ -2570,7 +2581,7 @@
       <c r="P37" s="32">
         <v>24</v>
       </c>
-      <c r="Q37" s="106"/>
+      <c r="Q37" s="70"/>
       <c r="R37" s="10"/>
       <c r="S37" s="10"/>
       <c r="T37" s="10"/>
@@ -2602,7 +2613,7 @@
       <c r="P38" s="34">
         <v>26</v>
       </c>
-      <c r="Q38" s="107"/>
+      <c r="Q38" s="71"/>
       <c r="R38" s="10"/>
       <c r="S38" s="10"/>
       <c r="T38" s="10"/>
@@ -3357,6 +3368,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A4:R7"/>
+    <mergeCell ref="L22:P22"/>
+    <mergeCell ref="L19:P21"/>
+    <mergeCell ref="N8:Q9"/>
+    <mergeCell ref="Q23:Q31"/>
+    <mergeCell ref="A23:A31"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="Q34:Q38"/>
     <mergeCell ref="J8:M9"/>
@@ -3373,12 +3390,6 @@
     <mergeCell ref="B19:F21"/>
     <mergeCell ref="G19:K21"/>
     <mergeCell ref="G32:K32"/>
-    <mergeCell ref="A4:R7"/>
-    <mergeCell ref="L22:P22"/>
-    <mergeCell ref="L19:P21"/>
-    <mergeCell ref="N8:Q9"/>
-    <mergeCell ref="Q23:Q31"/>
-    <mergeCell ref="A23:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>